<commit_message>
Fixed some f12018 motion data mappings
</commit_message>
<xml_diff>
--- a/telemetry/src/main/resources/f12018-mappings.xlsx
+++ b/telemetry/src/main/resources/f12018-mappings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\f1_wheel\telemetry\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD75101C-C4DF-47B2-AA26-90D74C5CB767}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CD385FB-FA4C-4B8A-9E6C-E5B798A4420F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8160" xr2:uid="{DCDA455C-B404-49E1-BDCA-B89DC0E9D2BA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8160" activeTab="2" xr2:uid="{DCDA455C-B404-49E1-BDCA-B89DC0E9D2BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Motion" sheetId="1" r:id="rId1"/>
@@ -632,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A747F35F-E4D2-4396-BA99-C565238D80A1}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1440,8 +1440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1508EF5F-74BE-427F-8E06-C02DB04FD999}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1544,6 +1544,10 @@
       <c r="F5">
         <v>1</v>
       </c>
+      <c r="G5">
+        <f t="shared" ref="G5:G16" si="0">G4+F4</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6">
@@ -1556,6 +1560,10 @@
       <c r="F6">
         <v>1</v>
       </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
@@ -1564,6 +1572,10 @@
       <c r="F7">
         <v>1</v>
       </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
@@ -1572,6 +1584,10 @@
       <c r="F8">
         <v>1</v>
       </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
@@ -1580,6 +1596,10 @@
       <c r="F9">
         <v>2</v>
       </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
@@ -1588,6 +1608,10 @@
       <c r="F10">
         <v>1</v>
       </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
@@ -1596,6 +1620,10 @@
       <c r="F11">
         <v>1</v>
       </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
@@ -1604,6 +1632,10 @@
       <c r="F12">
         <v>8</v>
       </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
@@ -1612,6 +1644,10 @@
       <c r="F13">
         <v>8</v>
       </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
@@ -1620,6 +1656,10 @@
       <c r="F14">
         <v>8</v>
       </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
@@ -1628,6 +1668,10 @@
       <c r="F15">
         <v>2</v>
       </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
@@ -1635,6 +1679,10 @@
       </c>
       <c r="F16">
         <v>16</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Workaround for f1 2018 bug where laps completed is actually +2 over the value it should be. In F12017  it was +1 over!
</commit_message>
<xml_diff>
--- a/telemetry/src/main/resources/f12018-mappings.xlsx
+++ b/telemetry/src/main/resources/f12018-mappings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\f1_wheel\telemetry\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CD385FB-FA4C-4B8A-9E6C-E5B798A4420F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49AD5EC-E416-4F1C-9535-202E11E13649}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8160" activeTab="2" xr2:uid="{DCDA455C-B404-49E1-BDCA-B89DC0E9D2BA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8160" xr2:uid="{DCDA455C-B404-49E1-BDCA-B89DC0E9D2BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Motion" sheetId="1" r:id="rId1"/>
@@ -312,10 +312,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -632,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A747F35F-E4D2-4396-BA99-C565238D80A1}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,40 +643,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="E1" s="1" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J2" s="1"/>
+      <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1144,35 +1144,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="1" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1440,7 +1440,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1508EF5F-74BE-427F-8E06-C02DB04FD999}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
@@ -1451,35 +1451,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="1" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>